<commit_message>
Criação Tabela de Horários
</commit_message>
<xml_diff>
--- a/CSV_2_XLSX.xlsx
+++ b/CSV_2_XLSX.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="33">
   <si>
     <t>Engenharia de Computação</t>
   </si>
@@ -140,7 +140,7 @@
       <patternFill patternType="darkGray"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -148,16 +148,87 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -176,7 +247,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="C1" t="s" s="1">
+      <c r="C1" t="s" s="3">
         <v>0</v>
       </c>
     </row>
@@ -278,6 +349,24 @@
       <c r="A18" t="s" s="2">
         <v>22</v>
       </c>
+      <c r="B18" t="s" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s" s="1">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s" s="1">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s" s="1">
+        <v>4</v>
+      </c>
+      <c r="F18" t="s" s="1">
+        <v>5</v>
+      </c>
+      <c r="G18" t="s" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="1">
@@ -354,6 +443,24 @@
       <c r="A34" t="s" s="2">
         <v>23</v>
       </c>
+      <c r="B34" t="s" s="1">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s" s="1">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s" s="1">
+        <v>3</v>
+      </c>
+      <c r="E34" t="s" s="1">
+        <v>4</v>
+      </c>
+      <c r="F34" t="s" s="1">
+        <v>5</v>
+      </c>
+      <c r="G34" t="s" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="1">
@@ -430,6 +537,24 @@
       <c r="A50" t="s" s="2">
         <v>24</v>
       </c>
+      <c r="B50" t="s" s="1">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s" s="1">
+        <v>2</v>
+      </c>
+      <c r="D50" t="s" s="1">
+        <v>3</v>
+      </c>
+      <c r="E50" t="s" s="1">
+        <v>4</v>
+      </c>
+      <c r="F50" t="s" s="1">
+        <v>5</v>
+      </c>
+      <c r="G50" t="s" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="1">
@@ -506,6 +631,24 @@
       <c r="A66" t="s" s="2">
         <v>25</v>
       </c>
+      <c r="B66" t="s" s="1">
+        <v>1</v>
+      </c>
+      <c r="C66" t="s" s="1">
+        <v>2</v>
+      </c>
+      <c r="D66" t="s" s="1">
+        <v>3</v>
+      </c>
+      <c r="E66" t="s" s="1">
+        <v>4</v>
+      </c>
+      <c r="F66" t="s" s="1">
+        <v>5</v>
+      </c>
+      <c r="G66" t="s" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="1">
@@ -582,6 +725,24 @@
       <c r="A82" t="s" s="2">
         <v>26</v>
       </c>
+      <c r="B82" t="s" s="1">
+        <v>1</v>
+      </c>
+      <c r="C82" t="s" s="1">
+        <v>2</v>
+      </c>
+      <c r="D82" t="s" s="1">
+        <v>3</v>
+      </c>
+      <c r="E82" t="s" s="1">
+        <v>4</v>
+      </c>
+      <c r="F82" t="s" s="1">
+        <v>5</v>
+      </c>
+      <c r="G82" t="s" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="s" s="1">
@@ -658,6 +819,24 @@
       <c r="A98" t="s" s="2">
         <v>27</v>
       </c>
+      <c r="B98" t="s" s="1">
+        <v>1</v>
+      </c>
+      <c r="C98" t="s" s="1">
+        <v>2</v>
+      </c>
+      <c r="D98" t="s" s="1">
+        <v>3</v>
+      </c>
+      <c r="E98" t="s" s="1">
+        <v>4</v>
+      </c>
+      <c r="F98" t="s" s="1">
+        <v>5</v>
+      </c>
+      <c r="G98" t="s" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="s" s="1">
@@ -734,6 +913,24 @@
       <c r="A114" t="s" s="2">
         <v>28</v>
       </c>
+      <c r="B114" t="s" s="1">
+        <v>1</v>
+      </c>
+      <c r="C114" t="s" s="1">
+        <v>2</v>
+      </c>
+      <c r="D114" t="s" s="1">
+        <v>3</v>
+      </c>
+      <c r="E114" t="s" s="1">
+        <v>4</v>
+      </c>
+      <c r="F114" t="s" s="1">
+        <v>5</v>
+      </c>
+      <c r="G114" t="s" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="s" s="1">
@@ -810,6 +1007,24 @@
       <c r="A130" t="s" s="2">
         <v>29</v>
       </c>
+      <c r="B130" t="s" s="1">
+        <v>1</v>
+      </c>
+      <c r="C130" t="s" s="1">
+        <v>2</v>
+      </c>
+      <c r="D130" t="s" s="1">
+        <v>3</v>
+      </c>
+      <c r="E130" t="s" s="1">
+        <v>4</v>
+      </c>
+      <c r="F130" t="s" s="1">
+        <v>5</v>
+      </c>
+      <c r="G130" t="s" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="s" s="1">
@@ -886,6 +1101,24 @@
       <c r="A146" t="s" s="2">
         <v>30</v>
       </c>
+      <c r="B146" t="s" s="1">
+        <v>1</v>
+      </c>
+      <c r="C146" t="s" s="1">
+        <v>2</v>
+      </c>
+      <c r="D146" t="s" s="1">
+        <v>3</v>
+      </c>
+      <c r="E146" t="s" s="1">
+        <v>4</v>
+      </c>
+      <c r="F146" t="s" s="1">
+        <v>5</v>
+      </c>
+      <c r="G146" t="s" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="s" s="1">
@@ -962,6 +1195,24 @@
       <c r="A162" t="s" s="2">
         <v>31</v>
       </c>
+      <c r="B162" t="s" s="1">
+        <v>1</v>
+      </c>
+      <c r="C162" t="s" s="1">
+        <v>2</v>
+      </c>
+      <c r="D162" t="s" s="1">
+        <v>3</v>
+      </c>
+      <c r="E162" t="s" s="1">
+        <v>4</v>
+      </c>
+      <c r="F162" t="s" s="1">
+        <v>5</v>
+      </c>
+      <c r="G162" t="s" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="s" s="1">
@@ -1037,6 +1288,24 @@
     <row r="178">
       <c r="A178" t="s" s="2">
         <v>32</v>
+      </c>
+      <c r="B178" t="s" s="1">
+        <v>1</v>
+      </c>
+      <c r="C178" t="s" s="1">
+        <v>2</v>
+      </c>
+      <c r="D178" t="s" s="1">
+        <v>3</v>
+      </c>
+      <c r="E178" t="s" s="1">
+        <v>4</v>
+      </c>
+      <c r="F178" t="s" s="1">
+        <v>5</v>
+      </c>
+      <c r="G178" t="s" s="1">
+        <v>6</v>
       </c>
     </row>
     <row r="179">

</xml_diff>

<commit_message>
Tabela de Horários FINALIZADA, faltam detalhe que não influenciam no final
</commit_message>
<xml_diff>
--- a/CSV_2_XLSX.xlsx
+++ b/CSV_2_XLSX.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="38">
   <si>
     <t>Engenharia de Computação</t>
   </si>
@@ -117,6 +117,15 @@
   </si>
   <si>
     <t>Engenharia Mecânica</t>
+  </si>
+  <si>
+    <t>dsc111|Prof026|12</t>
+  </si>
+  <si>
+    <t>dsc112|Prof043|8</t>
+  </si>
+  <si>
+    <t>dsc311|Prof096|27</t>
   </si>
 </sst>
 </file>
@@ -226,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
       <alignment horizontal="center" vertical="center"/>
@@ -235,6 +244,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -252,6 +264,9 @@
     <col min="1" max="1" width="11.73046875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="11.73046875" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="11.73046875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="18.55859375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="17.4453125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="18.55859375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -334,6 +349,9 @@
       <c r="A3" t="s" s="1">
         <v>7</v>
       </c>
+      <c r="D3" t="s" s="4">
+        <v>35</v>
+      </c>
       <c r="J3" t="s" s="1">
         <v>7</v>
       </c>
@@ -395,6 +413,9 @@
       <c r="S8" t="s" s="1">
         <v>12</v>
       </c>
+      <c r="Y8" t="s" s="4">
+        <v>37</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="1">
@@ -454,6 +475,9 @@
     <row r="14">
       <c r="A14" t="s" s="1">
         <v>18</v>
+      </c>
+      <c r="F14" t="s" s="4">
+        <v>36</v>
       </c>
       <c r="J14" t="s" s="1">
         <v>18</v>

</xml_diff>